<commit_message>
add tests for 0.63
</commit_message>
<xml_diff>
--- a/test/regression/xlsx_files/chart_errorbars07.xlsx
+++ b/test/regression/xlsx_files/chart_errorbars07.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="270" windowWidth="15855" windowHeight="9405"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$1:$A$5</c:f>
               <c:numCache>
-                <c:formatCode>dd/mm/yyyy</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>39083</c:v>
@@ -148,7 +148,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$1:$A$5</c:f>
               <c:numCache>
-                <c:formatCode>dd/mm/yyyy</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>39083</c:v>
@@ -214,7 +214,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$1:$A$5</c:f>
               <c:numCache>
-                <c:formatCode>dd/mm/yyyy</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>39083</c:v>
@@ -298,7 +298,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>

</xml_diff>